<commit_message>
Add Volume License Checking
</commit_message>
<xml_diff>
--- a/BUG_LIST.xlsx
+++ b/BUG_LIST.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="11 JAN 2017" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
   <si>
     <t>MASTER PRODUK</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>retur jual bukan berupa cash, tidak ada message kalau tidak ada bon lagi dari customer tersebut</t>
+  </si>
+  <si>
+    <t>hasil query untuk message lebih dari 1000</t>
   </si>
 </sst>
 </file>
@@ -437,7 +440,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
@@ -635,10 +638,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3"/>
+  <dimension ref="B3:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,6 +654,11 @@
         <v>24</v>
       </c>
     </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
UI Minor update and Bug Fix List Update
</commit_message>
<xml_diff>
--- a/BUG_LIST.xlsx
+++ b/BUG_LIST.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\RoyalPetz\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9435"/>
   </bookViews>
   <sheets>
     <sheet name="11 JAN 2017" sheetId="1" r:id="rId1"/>
     <sheet name="ALL MODULES" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
   <si>
     <t>MASTER PRODUK</t>
   </si>
@@ -118,6 +113,24 @@
   </si>
   <si>
     <t>retur jual bukan berupa cash, tidak ada message kalau tidak ada bon lagi dari customer tersebut</t>
+  </si>
+  <si>
+    <t>PEMBAYARAN PIUTANG PER-CUSTOMER</t>
+  </si>
+  <si>
+    <t>PEMBAYARAN PIUTANG PER-INVOICE</t>
+  </si>
+  <si>
+    <t>Pada saat save error mysqlexception unknown column ORIGIN_SALES_INVOICE</t>
+  </si>
+  <si>
+    <t>error nullreferenceexception pada prosedur unregisterglobalhotkey</t>
+  </si>
+  <si>
+    <t>PEMBAYARAN HUTANG PER-INVOICE</t>
+  </si>
+  <si>
+    <t>PEMBAYARAN HUTANG PER-CUSTOMER</t>
   </si>
 </sst>
 </file>
@@ -427,7 +440,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -435,15 +448,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D33"/>
+  <dimension ref="B1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:XFD40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="28.140625" customWidth="1"/>
+    <col min="2" max="2" width="36.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="87.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -620,12 +633,44 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>30</v>
       </c>
       <c r="D33" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>35</v>
+      </c>
+      <c r="C39" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Bug Fix and New DB Dump
</commit_message>
<xml_diff>
--- a/BUG_LIST.xlsx
+++ b/BUG_LIST.xlsx
@@ -1,14 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\RoyalPetz\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="11 JAN 2017" sheetId="1" r:id="rId1"/>
-    <sheet name="ALL MODULES" sheetId="2" r:id="rId2"/>
+    <sheet name="TODO" sheetId="3" r:id="rId2"/>
+    <sheet name="ALL MODULES" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -20,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="40">
   <si>
     <t>MASTER PRODUK</t>
   </si>
@@ -131,6 +137,15 @@
   </si>
   <si>
     <t>PEMBAYARAN HUTANG PER-CUSTOMER</t>
+  </si>
+  <si>
+    <t>TRANSAKSI JURNAL HARIAN</t>
+  </si>
+  <si>
+    <t>error null reference pada unregister global hotkey</t>
+  </si>
+  <si>
+    <t>Import and Export Data Mutasi with Expiry Date</t>
   </si>
 </sst>
 </file>
@@ -440,7 +455,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -448,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D41"/>
+  <dimension ref="B1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40:XFD40"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,6 +663,9 @@
       <c r="C35" t="s">
         <v>34</v>
       </c>
+      <c r="D35" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
@@ -664,6 +682,9 @@
       <c r="C39" t="s">
         <v>34</v>
       </c>
+      <c r="D39" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
@@ -671,6 +692,20 @@
       </c>
       <c r="C41" t="s">
         <v>34</v>
+      </c>
+      <c r="D41" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>37</v>
+      </c>
+      <c r="C43" t="s">
+        <v>38</v>
+      </c>
+      <c r="D43" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -679,6 +714,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="73" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3"/>
   <sheetViews>

</xml_diff>

<commit_message>
Add Changes on Volume License Checking
</commit_message>
<xml_diff>
--- a/BUG_LIST.xlsx
+++ b/BUG_LIST.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
   <si>
     <t>MASTER PRODUK</t>
   </si>
@@ -146,6 +146,12 @@
   </si>
   <si>
     <t>Import and Export Data Mutasi with Expiry Date</t>
+  </si>
+  <si>
+    <t>save volume license di folder baru di application data</t>
+  </si>
+  <si>
+    <t>Load Data Mutasi di Penerimaan Barang, untuk menampilkan tgl expiry</t>
   </si>
 </sst>
 </file>
@@ -465,7 +471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
@@ -715,7 +721,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3"/>
+  <dimension ref="B3:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
@@ -731,6 +737,16 @@
         <v>39</v>
       </c>
     </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -741,7 +757,7 @@
   <dimension ref="B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add Expiry Date to Import / Export Mutasi
</commit_message>
<xml_diff>
--- a/BUG_LIST.xlsx
+++ b/BUG_LIST.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
   <si>
     <t>MASTER PRODUK</t>
   </si>
@@ -472,7 +472,7 @@
   <dimension ref="B1:D43"/>
   <sheetViews>
     <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,10 +721,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:B5"/>
+  <dimension ref="B3:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,19 +732,28 @@
     <col min="2" max="2" width="73" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Revisi Nota (UNTESTED)
</commit_message>
<xml_diff>
--- a/BUG_LIST.xlsx
+++ b/BUG_LIST.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="46">
   <si>
     <t>MASTER PRODUK</t>
   </si>
@@ -152,14 +152,67 @@
   </si>
   <si>
     <t>Load Data Mutasi di Penerimaan Barang, untuk menampilkan tgl expiry</t>
+  </si>
+  <si>
+    <t>Simpan data orang yg mengedit sales order</t>
+  </si>
+  <si>
+    <t>Copy Nota menampilkan data orang yg mengedit sales order</t>
+  </si>
+  <si>
+    <r>
+      <t>Edit Sales Order</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>memanfaatkan copy nota</t>
+    </r>
+  </si>
+  <si>
+    <t>Tambah persenan untuk harga di master produk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -187,8 +240,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -721,10 +775,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:C5"/>
+  <dimension ref="B3:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,8 +810,29 @@
         <v>8</v>
       </c>
     </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>